<commit_message>
Update repo - 13/01:4.00PM
</commit_message>
<xml_diff>
--- a/Docs/AGV Project.xlsx
+++ b/Docs/AGV Project.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Dropbox\Works\AGV\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE950CE8-AFC5-43A2-B61C-75CD5DF3DF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F868F5A7-75B3-47FC-95E0-CD3A9685DC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="879" firstSheet="2" activeTab="5" xr2:uid="{3153E09C-E851-44BE-BE0B-53D6377AEEB6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="879" xr2:uid="{3153E09C-E851-44BE-BE0B-53D6377AEEB6}"/>
   </bookViews>
   <sheets>
     <sheet name="General Description" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -76,9 +75,6 @@
     <t>- AGV must be auto in finding path, avoiding collisions, finding charging station
 - System must ensure speed of transporting of robots associated with efficiency in moving
 - Not having expensive hardwares but still be efficient</t>
-  </si>
-  <si>
-    <t>Tech stacks</t>
   </si>
   <si>
     <t>Pricing</t>
@@ -210,6 +206,9 @@
 - Make software design diagram
 - Measure BLE signal strength and according receiving distance
 - Calculate basic positioning method base on BLE signal and laser data</t>
+  </si>
+  <si>
+    <t>Techs</t>
   </si>
 </sst>
 </file>
@@ -547,57 +546,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -613,13 +570,46 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -649,17 +639,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -18610,8 +18609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3CC26E-C741-4BA0-B87C-D3EE4B2AA9E5}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
@@ -18625,47 +18624,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="26" t="s">
-        <v>9</v>
+      <c r="D1" s="12" t="s">
+        <v>47</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="21"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" ht="324.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="22"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18683,139 +18682,139 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" style="40" customWidth="1"/>
-    <col min="2" max="2" width="28.5546875" style="40" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" style="40" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" style="40" customWidth="1"/>
-    <col min="5" max="5" width="19" style="40" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="40"/>
+    <col min="1" max="1" width="18.33203125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="28.5546875" style="14" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="19" style="14" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="39" t="s">
+      <c r="E1" s="13" t="s">
         <v>35</v>
-      </c>
-      <c r="D1" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="169.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="42" t="s">
-        <v>41</v>
+      <c r="C2" s="16" t="s">
+        <v>46</v>
       </c>
-      <c r="C2" s="42" t="s">
-        <v>47</v>
+      <c r="D2" s="15" t="s">
+        <v>42</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="E2" s="15" t="s">
         <v>43</v>
-      </c>
-      <c r="E2" s="41" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="188.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="41" t="s">
-        <v>39</v>
+      <c r="A3" s="15" t="s">
+        <v>38</v>
       </c>
-      <c r="B3" s="42" t="s">
-        <v>42</v>
+      <c r="B3" s="16" t="s">
+        <v>41</v>
       </c>
-      <c r="C3" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="41" t="s">
+      <c r="C3" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="41"/>
+      <c r="D3" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="15"/>
     </row>
     <row r="4" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="41"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
     </row>
     <row r="5" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="41"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
     </row>
     <row r="6" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="41"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
     </row>
     <row r="7" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="41"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
     </row>
     <row r="8" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="41"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
     </row>
     <row r="9" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="41"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
     </row>
     <row r="10" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="41"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="41"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
     </row>
     <row r="12" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
     </row>
     <row r="13" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="41"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="41"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18832,10 +18831,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="16384" width="8.88671875" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:XFD1048576"/>
@@ -18856,7 +18855,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="16384" width="8.88671875" style="18"/>
   </cols>
   <sheetData/>
   <mergeCells count="1">
@@ -18878,272 +18877,266 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.77734375" style="13" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" style="13" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="13"/>
-    <col min="7" max="7" width="20.21875" style="13" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" style="13" customWidth="1"/>
-    <col min="10" max="10" width="14.21875" style="13" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="13" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="13"/>
+    <col min="1" max="1" width="22.77734375" style="21" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" style="21" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" style="21" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="21" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" style="21" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="21"/>
+    <col min="7" max="7" width="20.21875" style="21" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" style="21" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" style="21" customWidth="1"/>
+    <col min="10" max="10" width="14.21875" style="21" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="21" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="11" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:12" s="19" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="27" t="s">
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="38"/>
+    </row>
+    <row r="2" spans="1:12" s="19" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="40"/>
+      <c r="G2" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="29"/>
+      <c r="J2" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="20"/>
+    </row>
+    <row r="3" spans="1:12" s="19" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="27"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="20"/>
+    </row>
+    <row r="4" spans="1:12" s="19" customFormat="1" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="24"/>
+      <c r="B4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="29"/>
-    </row>
-    <row r="2" spans="1:12" s="11" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
-        <v>2</v>
+      <c r="C4" s="4" t="s">
+        <v>13</v>
       </c>
-      <c r="B2" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="19" t="s">
+      <c r="D4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="17" t="s">
-        <v>2</v>
+      <c r="E4" s="6" t="s">
+        <v>17</v>
       </c>
-      <c r="H2" s="31" t="s">
-        <v>10</v>
+      <c r="F4" s="40"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="6" t="s">
+        <v>12</v>
       </c>
-      <c r="I2" s="32"/>
-      <c r="J2" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="12"/>
-    </row>
-    <row r="3" spans="1:12" s="11" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="30"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="12"/>
-    </row>
-    <row r="4" spans="1:12" s="11" customFormat="1" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="18"/>
-      <c r="B4" s="16" t="s">
+      <c r="I4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>14</v>
+      <c r="J4" s="6" t="s">
+        <v>26</v>
       </c>
-      <c r="D4" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="16" t="s">
+      <c r="K4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="16" t="s">
-        <v>13</v>
+      <c r="L4" s="20"/>
+    </row>
+    <row r="5" spans="1:12" s="19" customFormat="1" ht="156.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>29</v>
       </c>
-      <c r="I4" s="7" t="s">
-        <v>14</v>
+      <c r="B5" s="6" t="s">
+        <v>20</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="C5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="20"/>
+    </row>
+    <row r="6" spans="1:12" s="19" customFormat="1" ht="111" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="I6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="20"/>
+    </row>
+    <row r="7" spans="1:12" s="19" customFormat="1" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="12"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="20"/>
     </row>
-    <row r="5" spans="1:12" s="11" customFormat="1" ht="156.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="12"/>
+    <row r="8" spans="1:12" s="19" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="20"/>
     </row>
-    <row r="6" spans="1:12" s="11" customFormat="1" ht="111" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="12"/>
+    <row r="9" spans="1:12" s="19" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="20"/>
     </row>
-    <row r="7" spans="1:12" s="11" customFormat="1" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="12"/>
+    <row r="10" spans="1:12" s="19" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="3"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="20"/>
     </row>
-    <row r="8" spans="1:12" s="11" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="12"/>
+    <row r="11" spans="1:12" s="19" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="3"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="20"/>
     </row>
-    <row r="9" spans="1:12" s="11" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="12"/>
-    </row>
-    <row r="10" spans="1:12" s="11" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="6"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="12"/>
-    </row>
-    <row r="11" spans="1:12" s="11" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="6"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="12"/>
-    </row>
-    <row r="12" spans="1:12" s="11" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="6"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="12"/>
+    <row r="12" spans="1:12" s="19" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="3"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="20"/>
     </row>
     <row r="13" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="H2:I3"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="F1:F12"/>
     <mergeCell ref="L1:XFD12"/>
     <mergeCell ref="A13:XFD1048576"/>
     <mergeCell ref="J2:J3"/>
@@ -19151,6 +19144,12 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="G2:G4"/>
+    <mergeCell ref="H2:I3"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="F1:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -19161,16 +19160,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FFB7DAA-B4A5-4CCA-8A25-F20A0F718CEB}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="16384" width="8.88671875" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:XFD1048576"/>
@@ -19190,10 +19189,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="16384" width="8.88671875" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:XFD1048576"/>
@@ -19212,10 +19211,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="16384" width="8.88671875" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:XFD1048576"/>
@@ -19234,7 +19233,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="5"/>
+    <col min="1" max="16384" width="8.88671875" style="42"/>
   </cols>
   <sheetData/>
   <mergeCells count="1">

</xml_diff>